<commit_message>
Minor changes to logo, titles, and font size.
</commit_message>
<xml_diff>
--- a/data/etc/2015/duplicates.xlsx
+++ b/data/etc/2015/duplicates.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250128" uniqueCount="2546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260550" uniqueCount="2546">
   <si>
     <t>submissiondate</t>
   </si>
@@ -11129,13 +11129,13 @@
         <v>180</v>
       </c>
       <c r="B12" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C12" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
         <v>403</v>
@@ -11176,7 +11176,7 @@
         <v>1</v>
       </c>
       <c r="S12" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="T12" s="0">
         <v>6</v>
@@ -11200,31 +11200,31 @@
         <v>3</v>
       </c>
       <c r="AA12" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="AB12" t="s">
         <v>619</v>
       </c>
       <c r="AC12" s="0">
+        <v>61973012</v>
+      </c>
+      <c r="AD12" s="0">
         <v>79062914</v>
       </c>
-      <c r="AD12" s="0">
-        <v>61973012</v>
-      </c>
       <c r="AE12" s="0">
-        <v>13.063042640686035</v>
+        <v>13.076375961303711</v>
       </c>
       <c r="AF12" s="0">
-        <v>-1.0849522352218628</v>
+        <v>-1.086039662361145</v>
       </c>
       <c r="AG12" s="0">
-        <v>354.53817749023437</v>
+        <v>342.7674560546875</v>
       </c>
       <c r="AH12" s="0">
         <v>4</v>
       </c>
       <c r="AI12" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="AJ12" t="s">
         <v>731</v>
@@ -11233,7 +11233,7 @@
         <v>72016</v>
       </c>
       <c r="AL12" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="AM12" s="0">
         <v>1</v>
@@ -11247,13 +11247,13 @@
         <v>180</v>
       </c>
       <c r="B13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
         <v>403</v>
@@ -11294,7 +11294,7 @@
         <v>1</v>
       </c>
       <c r="S13" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="T13" s="0">
         <v>6</v>
@@ -11318,31 +11318,31 @@
         <v>3</v>
       </c>
       <c r="AA13" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="AB13" t="s">
         <v>619</v>
       </c>
       <c r="AC13" s="0">
+        <v>79062914</v>
+      </c>
+      <c r="AD13" s="0">
         <v>61973012</v>
       </c>
-      <c r="AD13" s="0">
-        <v>79062914</v>
-      </c>
       <c r="AE13" s="0">
-        <v>13.076375961303711</v>
+        <v>13.063042640686035</v>
       </c>
       <c r="AF13" s="0">
-        <v>-1.086039662361145</v>
+        <v>-1.0849522352218628</v>
       </c>
       <c r="AG13" s="0">
-        <v>342.7674560546875</v>
+        <v>354.53817749023437</v>
       </c>
       <c r="AH13" s="0">
         <v>4</v>
       </c>
       <c r="AI13" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AJ13" t="s">
         <v>731</v>
@@ -11351,7 +11351,7 @@
         <v>72016</v>
       </c>
       <c r="AL13" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AM13" s="0">
         <v>1</v>
@@ -12771,10 +12771,10 @@
         <v>190</v>
       </c>
       <c r="B26" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C26" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D26" t="s">
         <v>397</v>
@@ -12798,13 +12798,13 @@
         <v>89</v>
       </c>
       <c r="K26" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="L26" s="0">
-        <v>71183878</v>
+        <v>69153400</v>
       </c>
       <c r="M26" s="0">
-        <v>71183878</v>
+        <v>69153400</v>
       </c>
       <c r="N26" s="0"/>
       <c r="O26" s="0">
@@ -12812,35 +12812,37 @@
       </c>
       <c r="P26" s="0"/>
       <c r="Q26" s="0">
+        <v>6</v>
+      </c>
+      <c r="R26" s="0">
+        <v>1</v>
+      </c>
+      <c r="S26" s="0">
+        <v>9</v>
+      </c>
+      <c r="T26" s="0">
+        <v>0</v>
+      </c>
+      <c r="U26" s="0">
+        <v>0</v>
+      </c>
+      <c r="V26" s="0">
+        <v>1</v>
+      </c>
+      <c r="W26" s="0">
+        <v>0</v>
+      </c>
+      <c r="X26" t="s">
+        <v>569</v>
+      </c>
+      <c r="Y26" s="0">
+        <v>2</v>
+      </c>
+      <c r="Z26" s="0">
         <v>3</v>
       </c>
-      <c r="R26" s="0">
-        <v>0</v>
-      </c>
-      <c r="S26" s="0"/>
-      <c r="T26" s="0">
-        <v>6</v>
-      </c>
-      <c r="U26" s="0">
-        <v>6</v>
-      </c>
-      <c r="V26" s="0">
-        <v>1</v>
-      </c>
-      <c r="W26" s="0">
-        <v>0</v>
-      </c>
-      <c r="X26" t="s">
-        <v>570</v>
-      </c>
-      <c r="Y26" s="0">
-        <v>1</v>
-      </c>
-      <c r="Z26" s="0">
-        <v>4</v>
-      </c>
       <c r="AA26" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="AB26" t="s">
         <v>623</v>
@@ -12852,19 +12854,19 @@
         <v>76258561</v>
       </c>
       <c r="AE26" s="0">
-        <v>12.182738304138184</v>
+        <v>12.182742118835449</v>
       </c>
       <c r="AF26" s="0">
-        <v>-1.555014967918396</v>
+        <v>-1.5550111532211304</v>
       </c>
       <c r="AG26" s="0">
-        <v>332.791015625</v>
+        <v>334.52459716796875</v>
       </c>
       <c r="AH26" s="0">
         <v>4</v>
       </c>
       <c r="AI26" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="AJ26" t="s">
         <v>738</v>
@@ -12873,7 +12875,7 @@
         <v>72016</v>
       </c>
       <c r="AL26" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="AM26" s="0">
         <v>1</v>
@@ -12887,10 +12889,10 @@
         <v>190</v>
       </c>
       <c r="B27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D27" t="s">
         <v>397</v>
@@ -12914,13 +12916,13 @@
         <v>89</v>
       </c>
       <c r="K27" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L27" s="0">
-        <v>69153400</v>
+        <v>71183878</v>
       </c>
       <c r="M27" s="0">
-        <v>69153400</v>
+        <v>71183878</v>
       </c>
       <c r="N27" s="0"/>
       <c r="O27" s="0">
@@ -12928,19 +12930,17 @@
       </c>
       <c r="P27" s="0"/>
       <c r="Q27" s="0">
+        <v>3</v>
+      </c>
+      <c r="R27" s="0">
+        <v>0</v>
+      </c>
+      <c r="S27" s="0"/>
+      <c r="T27" s="0">
         <v>6</v>
       </c>
-      <c r="R27" s="0">
-        <v>1</v>
-      </c>
-      <c r="S27" s="0">
-        <v>9</v>
-      </c>
-      <c r="T27" s="0">
-        <v>0</v>
-      </c>
       <c r="U27" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="V27" s="0">
         <v>1</v>
@@ -12949,16 +12949,16 @@
         <v>0</v>
       </c>
       <c r="X27" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="Y27" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z27" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AA27" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="AB27" t="s">
         <v>623</v>
@@ -12970,19 +12970,19 @@
         <v>76258561</v>
       </c>
       <c r="AE27" s="0">
-        <v>12.182742118835449</v>
+        <v>12.182738304138184</v>
       </c>
       <c r="AF27" s="0">
-        <v>-1.5550111532211304</v>
+        <v>-1.555014967918396</v>
       </c>
       <c r="AG27" s="0">
-        <v>334.52459716796875</v>
+        <v>332.791015625</v>
       </c>
       <c r="AH27" s="0">
         <v>4</v>
       </c>
       <c r="AI27" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="AJ27" t="s">
         <v>738</v>
@@ -12991,7 +12991,7 @@
         <v>72016</v>
       </c>
       <c r="AL27" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="AM27" s="0">
         <v>1</v>
@@ -14175,10 +14175,10 @@
         <v>200</v>
       </c>
       <c r="B38" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C38" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D38" t="s">
         <v>399</v>
@@ -14258,19 +14258,19 @@
         <v>79542523</v>
       </c>
       <c r="AE38" s="0">
-        <v>12.363276481628418</v>
+        <v>12.363286972045898</v>
       </c>
       <c r="AF38" s="0">
-        <v>-1.4718724489212036</v>
+        <v>-1.4718532562255859</v>
       </c>
       <c r="AG38" s="0">
-        <v>334.67276000976562</v>
+        <v>310.28335571289062</v>
       </c>
       <c r="AH38" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AI38" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="AJ38" t="s">
         <v>744</v>
@@ -14279,7 +14279,7 @@
         <v>72016</v>
       </c>
       <c r="AL38" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="AM38" s="0">
         <v>1</v>
@@ -14293,10 +14293,10 @@
         <v>200</v>
       </c>
       <c r="B39" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C39" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D39" t="s">
         <v>399</v>
@@ -14376,19 +14376,19 @@
         <v>79542523</v>
       </c>
       <c r="AE39" s="0">
-        <v>12.363286972045898</v>
+        <v>12.363276481628418</v>
       </c>
       <c r="AF39" s="0">
-        <v>-1.4718532562255859</v>
+        <v>-1.4718724489212036</v>
       </c>
       <c r="AG39" s="0">
-        <v>310.28335571289062</v>
+        <v>334.67276000976562</v>
       </c>
       <c r="AH39" s="0">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AI39" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="AJ39" t="s">
         <v>744</v>
@@ -14397,7 +14397,7 @@
         <v>72016</v>
       </c>
       <c r="AL39" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="AM39" s="0">
         <v>1</v>
@@ -17829,13 +17829,13 @@
         <v>223</v>
       </c>
       <c r="B69" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C69" t="s">
-        <v>375</v>
+        <v>282</v>
       </c>
       <c r="D69" t="s">
-        <v>396</v>
+        <v>50</v>
       </c>
       <c r="E69" t="s">
         <v>411</v>
@@ -17856,7 +17856,7 @@
         <v>89</v>
       </c>
       <c r="K69" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="L69" s="0">
         <v>61151687</v>
@@ -17891,10 +17891,10 @@
         <v>0</v>
       </c>
       <c r="X69" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="Y69" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z69" s="0">
         <v>2</v>
@@ -17912,19 +17912,19 @@
         <v>70746732</v>
       </c>
       <c r="AE69" s="0">
-        <v>14.028984069824219</v>
+        <v>14.033792495727539</v>
       </c>
       <c r="AF69" s="0">
-        <v>-0.032648671418428421</v>
+        <v>-0.031043209135532379</v>
       </c>
       <c r="AG69" s="0">
-        <v>301.60000610351562</v>
+        <v>302.79998779296875</v>
       </c>
       <c r="AH69" s="0">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AI69" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="AJ69" t="s">
         <v>759</v>
@@ -17933,7 +17933,7 @@
         <v>72016</v>
       </c>
       <c r="AL69" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="AM69" s="0">
         <v>1</v>
@@ -17947,13 +17947,13 @@
         <v>223</v>
       </c>
       <c r="B70" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C70" t="s">
-        <v>282</v>
+        <v>375</v>
       </c>
       <c r="D70" t="s">
-        <v>50</v>
+        <v>396</v>
       </c>
       <c r="E70" t="s">
         <v>411</v>
@@ -17974,7 +17974,7 @@
         <v>89</v>
       </c>
       <c r="K70" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="L70" s="0">
         <v>61151687</v>
@@ -18009,10 +18009,10 @@
         <v>0</v>
       </c>
       <c r="X70" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="Y70" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z70" s="0">
         <v>2</v>
@@ -18030,19 +18030,19 @@
         <v>70746732</v>
       </c>
       <c r="AE70" s="0">
-        <v>14.033792495727539</v>
+        <v>14.028984069824219</v>
       </c>
       <c r="AF70" s="0">
-        <v>-0.031043209135532379</v>
+        <v>-0.032648671418428421</v>
       </c>
       <c r="AG70" s="0">
-        <v>302.79998779296875</v>
+        <v>301.60000610351562</v>
       </c>
       <c r="AH70" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI70" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="AJ70" t="s">
         <v>759</v>
@@ -18051,7 +18051,7 @@
         <v>72016</v>
       </c>
       <c r="AL70" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="AM70" s="0">
         <v>1</v>
@@ -18065,13 +18065,13 @@
         <v>222</v>
       </c>
       <c r="B71" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C71" t="s">
-        <v>288</v>
+        <v>376</v>
       </c>
       <c r="D71" t="s">
-        <v>396</v>
+        <v>50</v>
       </c>
       <c r="E71" t="s">
         <v>411</v>
@@ -18127,16 +18127,16 @@
         <v>0</v>
       </c>
       <c r="X71" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="Y71" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z71" s="0">
         <v>3</v>
       </c>
       <c r="AA71" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AB71" t="s">
         <v>633</v>
@@ -18148,19 +18148,19 @@
         <v>70746732</v>
       </c>
       <c r="AE71" s="0">
-        <v>14.029053688049316</v>
+        <v>14.033783912658691</v>
       </c>
       <c r="AF71" s="0">
-        <v>-0.03261445090174675</v>
+        <v>-0.031044170260429382</v>
       </c>
       <c r="AG71" s="0">
-        <v>308.5</v>
+        <v>303.79998779296875</v>
       </c>
       <c r="AH71" s="0">
         <v>5</v>
       </c>
       <c r="AI71" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="AJ71" t="s">
         <v>760</v>
@@ -18169,7 +18169,7 @@
         <v>72016</v>
       </c>
       <c r="AL71" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="AM71" s="0">
         <v>1</v>
@@ -18183,13 +18183,13 @@
         <v>222</v>
       </c>
       <c r="B72" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C72" t="s">
-        <v>376</v>
+        <v>288</v>
       </c>
       <c r="D72" t="s">
-        <v>50</v>
+        <v>396</v>
       </c>
       <c r="E72" t="s">
         <v>411</v>
@@ -18245,16 +18245,16 @@
         <v>0</v>
       </c>
       <c r="X72" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="Y72" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z72" s="0">
         <v>3</v>
       </c>
       <c r="AA72" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="AB72" t="s">
         <v>633</v>
@@ -18266,19 +18266,19 @@
         <v>70746732</v>
       </c>
       <c r="AE72" s="0">
-        <v>14.033783912658691</v>
+        <v>14.029053688049316</v>
       </c>
       <c r="AF72" s="0">
-        <v>-0.031044170260429382</v>
+        <v>-0.03261445090174675</v>
       </c>
       <c r="AG72" s="0">
-        <v>303.79998779296875</v>
+        <v>308.5</v>
       </c>
       <c r="AH72" s="0">
         <v>5</v>
       </c>
       <c r="AI72" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="AJ72" t="s">
         <v>760</v>
@@ -18287,7 +18287,7 @@
         <v>72016</v>
       </c>
       <c r="AL72" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="AM72" s="0">
         <v>1</v>
@@ -25853,13 +25853,13 @@
         <v>782</v>
       </c>
       <c r="B57" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C57" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="D57" t="s">
-        <v>45</v>
+        <v>396</v>
       </c>
       <c r="E57" t="s">
         <v>411</v>
@@ -25886,7 +25886,7 @@
         <v>1125</v>
       </c>
       <c r="M57" s="0">
-        <v>79664235</v>
+        <v>71296557</v>
       </c>
       <c r="N57" s="0">
         <v>79664235</v>
@@ -25897,13 +25897,13 @@
       </c>
       <c r="Q57" s="0"/>
       <c r="R57" s="0">
+        <v>2</v>
+      </c>
+      <c r="S57" s="0">
+        <v>1</v>
+      </c>
+      <c r="T57" s="0">
         <v>5</v>
-      </c>
-      <c r="S57" s="0">
-        <v>1</v>
-      </c>
-      <c r="T57" s="0">
-        <v>7</v>
       </c>
       <c r="U57" t="s">
         <v>633</v>
@@ -25915,19 +25915,19 @@
         <v>70746732</v>
       </c>
       <c r="X57" s="0">
-        <v>14.036609649658203</v>
+        <v>14.029008865356445</v>
       </c>
       <c r="Y57" s="0">
-        <v>-0.032943520694971085</v>
+        <v>-0.032592598348855972</v>
       </c>
       <c r="Z57" s="0">
-        <v>313.60000610351562</v>
+        <v>312.10000610351562</v>
       </c>
       <c r="AA57" s="0">
         <v>5</v>
       </c>
       <c r="AB57" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="AC57" t="s">
         <v>1320</v>
@@ -25936,7 +25936,7 @@
         <v>72016</v>
       </c>
       <c r="AE57" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="AF57" s="0">
         <v>3</v>
@@ -25950,13 +25950,13 @@
         <v>782</v>
       </c>
       <c r="B58" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C58" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="D58" t="s">
-        <v>396</v>
+        <v>45</v>
       </c>
       <c r="E58" t="s">
         <v>411</v>
@@ -25983,7 +25983,7 @@
         <v>1125</v>
       </c>
       <c r="M58" s="0">
-        <v>71296557</v>
+        <v>79664235</v>
       </c>
       <c r="N58" s="0">
         <v>79664235</v>
@@ -25994,13 +25994,13 @@
       </c>
       <c r="Q58" s="0"/>
       <c r="R58" s="0">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S58" s="0">
         <v>1</v>
       </c>
       <c r="T58" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="U58" t="s">
         <v>633</v>
@@ -26012,19 +26012,19 @@
         <v>70746732</v>
       </c>
       <c r="X58" s="0">
-        <v>14.029008865356445</v>
+        <v>14.036609649658203</v>
       </c>
       <c r="Y58" s="0">
-        <v>-0.032592598348855972</v>
+        <v>-0.032943520694971085</v>
       </c>
       <c r="Z58" s="0">
-        <v>312.10000610351562</v>
+        <v>313.60000610351562</v>
       </c>
       <c r="AA58" s="0">
         <v>5</v>
       </c>
       <c r="AB58" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="AC58" t="s">
         <v>1320</v>
@@ -26033,7 +26033,7 @@
         <v>72016</v>
       </c>
       <c r="AE58" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="AF58" s="0">
         <v>3</v>
@@ -26047,13 +26047,13 @@
         <v>776</v>
       </c>
       <c r="B59" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C59" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="D59" t="s">
-        <v>45</v>
+        <v>396</v>
       </c>
       <c r="E59" t="s">
         <v>411</v>
@@ -26080,10 +26080,10 @@
         <v>1125</v>
       </c>
       <c r="M59" s="0">
+        <v>71296557</v>
+      </c>
+      <c r="N59" s="0">
         <v>79664235</v>
-      </c>
-      <c r="N59" s="0">
-        <v>71296557</v>
       </c>
       <c r="O59" s="0"/>
       <c r="P59" s="0">
@@ -26091,13 +26091,13 @@
       </c>
       <c r="Q59" s="0"/>
       <c r="R59" s="0">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S59" s="0">
         <v>0</v>
       </c>
       <c r="T59" s="0">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="U59" t="s">
         <v>633</v>
@@ -26109,19 +26109,19 @@
         <v>70746732</v>
       </c>
       <c r="X59" s="0">
-        <v>14.036609649658203</v>
+        <v>14.029008865356445</v>
       </c>
       <c r="Y59" s="0">
-        <v>-0.032943520694971085</v>
+        <v>-0.032592598348855972</v>
       </c>
       <c r="Z59" s="0">
-        <v>313.60000610351562</v>
+        <v>312.10000610351562</v>
       </c>
       <c r="AA59" s="0">
         <v>5</v>
       </c>
       <c r="AB59" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="AC59" t="s">
         <v>1320</v>
@@ -26130,7 +26130,7 @@
         <v>72016</v>
       </c>
       <c r="AE59" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="AF59" s="0">
         <v>3</v>
@@ -26144,13 +26144,13 @@
         <v>776</v>
       </c>
       <c r="B60" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C60" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="D60" t="s">
-        <v>396</v>
+        <v>45</v>
       </c>
       <c r="E60" t="s">
         <v>411</v>
@@ -26177,10 +26177,10 @@
         <v>1125</v>
       </c>
       <c r="M60" s="0">
+        <v>79664235</v>
+      </c>
+      <c r="N60" s="0">
         <v>71296557</v>
-      </c>
-      <c r="N60" s="0">
-        <v>79664235</v>
       </c>
       <c r="O60" s="0"/>
       <c r="P60" s="0">
@@ -26188,13 +26188,13 @@
       </c>
       <c r="Q60" s="0"/>
       <c r="R60" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S60" s="0">
         <v>0</v>
       </c>
       <c r="T60" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="U60" t="s">
         <v>633</v>
@@ -26206,19 +26206,19 @@
         <v>70746732</v>
       </c>
       <c r="X60" s="0">
-        <v>14.029008865356445</v>
+        <v>14.036609649658203</v>
       </c>
       <c r="Y60" s="0">
-        <v>-0.032592598348855972</v>
+        <v>-0.032943520694971085</v>
       </c>
       <c r="Z60" s="0">
-        <v>312.10000610351562</v>
+        <v>313.60000610351562</v>
       </c>
       <c r="AA60" s="0">
         <v>5</v>
       </c>
       <c r="AB60" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="AC60" t="s">
         <v>1320</v>
@@ -26227,7 +26227,7 @@
         <v>72016</v>
       </c>
       <c r="AE60" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="AF60" s="0">
         <v>3</v>
@@ -32055,10 +32055,10 @@
         <v>775</v>
       </c>
       <c r="B121" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="C121" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="D121" t="s">
         <v>46</v>
@@ -32085,13 +32085,13 @@
         <v>89</v>
       </c>
       <c r="L121" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="M121" s="0">
-        <v>76493199</v>
+        <v>68463775</v>
       </c>
       <c r="N121" s="0">
-        <v>76493199</v>
+        <v>68463775</v>
       </c>
       <c r="O121" s="0"/>
       <c r="P121" s="0">
@@ -32105,7 +32105,7 @@
         <v>0</v>
       </c>
       <c r="T121" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U121" t="s">
         <v>130</v>
@@ -32117,19 +32117,19 @@
         <v>79146080</v>
       </c>
       <c r="X121" s="0">
-        <v>10.663491249084473</v>
+        <v>10.663528442382813</v>
       </c>
       <c r="Y121" s="0">
-        <v>-4.7367987632751465</v>
+        <v>-4.7367877960205078</v>
       </c>
       <c r="Z121" s="0">
-        <v>347.54165649414062</v>
+        <v>329.90121459960937</v>
       </c>
       <c r="AA121" s="0">
         <v>4</v>
       </c>
       <c r="AB121" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="AC121" t="s">
         <v>1341</v>
@@ -32138,7 +32138,7 @@
         <v>72016</v>
       </c>
       <c r="AE121" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="AF121" s="0">
         <v>1</v>
@@ -32152,10 +32152,10 @@
         <v>775</v>
       </c>
       <c r="B122" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="C122" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="D122" t="s">
         <v>46</v>
@@ -32182,13 +32182,13 @@
         <v>89</v>
       </c>
       <c r="L122" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="M122" s="0">
-        <v>68463775</v>
+        <v>76493199</v>
       </c>
       <c r="N122" s="0">
-        <v>68463775</v>
+        <v>76493199</v>
       </c>
       <c r="O122" s="0"/>
       <c r="P122" s="0">
@@ -32202,7 +32202,7 @@
         <v>0</v>
       </c>
       <c r="T122" s="0">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U122" t="s">
         <v>130</v>
@@ -32214,19 +32214,19 @@
         <v>79146080</v>
       </c>
       <c r="X122" s="0">
-        <v>10.663528442382813</v>
+        <v>10.663491249084473</v>
       </c>
       <c r="Y122" s="0">
-        <v>-4.7367877960205078</v>
+        <v>-4.7367987632751465</v>
       </c>
       <c r="Z122" s="0">
-        <v>329.90121459960937</v>
+        <v>347.54165649414062</v>
       </c>
       <c r="AA122" s="0">
         <v>4</v>
       </c>
       <c r="AB122" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="AC122" t="s">
         <v>1341</v>
@@ -32235,7 +32235,7 @@
         <v>72016</v>
       </c>
       <c r="AE122" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="AF122" s="0">
         <v>1</v>

</xml_diff>

<commit_message>
Update school well calculations.
</commit_message>
<xml_diff>
--- a/data/etc/2015/duplicates.xlsx
+++ b/data/etc/2015/duplicates.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302238" uniqueCount="2546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312660" uniqueCount="2546">
   <si>
     <t>submissiondate</t>
   </si>
@@ -14411,10 +14411,10 @@
         <v>201</v>
       </c>
       <c r="B40" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C40" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D40" t="s">
         <v>397</v>
@@ -14438,7 +14438,7 @@
         <v>89</v>
       </c>
       <c r="K40" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="L40" s="0">
         <v>76177548</v>
@@ -14458,7 +14458,7 @@
         <v>1</v>
       </c>
       <c r="S40" s="0">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="T40" s="0">
         <v>4</v>
@@ -14482,7 +14482,7 @@
         <v>3</v>
       </c>
       <c r="AA40" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="AB40" t="s">
         <v>623</v>
@@ -14494,19 +14494,19 @@
         <v>71261266</v>
       </c>
       <c r="AE40" s="0">
-        <v>12.182655334472656</v>
+        <v>12.182876586914063</v>
       </c>
       <c r="AF40" s="0">
-        <v>-1.5550374984741211</v>
+        <v>-1.5550318956375122</v>
       </c>
       <c r="AG40" s="0">
-        <v>330.74627685546875</v>
+        <v>339.3597412109375</v>
       </c>
       <c r="AH40" s="0">
         <v>4</v>
       </c>
       <c r="AI40" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="AJ40" t="s">
         <v>745</v>
@@ -14515,7 +14515,7 @@
         <v>72016</v>
       </c>
       <c r="AL40" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="AM40" s="0">
         <v>1</v>
@@ -14529,10 +14529,10 @@
         <v>201</v>
       </c>
       <c r="B41" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C41" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D41" t="s">
         <v>397</v>
@@ -14556,7 +14556,7 @@
         <v>89</v>
       </c>
       <c r="K41" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L41" s="0">
         <v>76177548</v>
@@ -14576,7 +14576,7 @@
         <v>1</v>
       </c>
       <c r="S41" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="T41" s="0">
         <v>4</v>
@@ -14600,7 +14600,7 @@
         <v>3</v>
       </c>
       <c r="AA41" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="AB41" t="s">
         <v>623</v>
@@ -14612,19 +14612,19 @@
         <v>71261266</v>
       </c>
       <c r="AE41" s="0">
-        <v>12.182876586914063</v>
+        <v>12.182655334472656</v>
       </c>
       <c r="AF41" s="0">
-        <v>-1.5550318956375122</v>
+        <v>-1.5550374984741211</v>
       </c>
       <c r="AG41" s="0">
-        <v>339.3597412109375</v>
+        <v>330.74627685546875</v>
       </c>
       <c r="AH41" s="0">
         <v>4</v>
       </c>
       <c r="AI41" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="AJ41" t="s">
         <v>745</v>
@@ -14633,7 +14633,7 @@
         <v>72016</v>
       </c>
       <c r="AL41" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="AM41" s="0">
         <v>1</v>
@@ -17361,13 +17361,13 @@
         <v>222</v>
       </c>
       <c r="B65" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C65" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D65" t="s">
-        <v>396</v>
+        <v>50</v>
       </c>
       <c r="E65" t="s">
         <v>411</v>
@@ -17424,13 +17424,13 @@
         <v>571</v>
       </c>
       <c r="Y65" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z65" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA65" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="AB65" t="s">
         <v>633</v>
@@ -17442,19 +17442,19 @@
         <v>70746732</v>
       </c>
       <c r="AE65" s="0">
-        <v>14.029009819030762</v>
+        <v>14.033710479736328</v>
       </c>
       <c r="AF65" s="0">
-        <v>-0.032633930444717407</v>
+        <v>-0.031045390293002129</v>
       </c>
       <c r="AG65" s="0">
-        <v>304.89999389648438</v>
+        <v>301.39999389648437</v>
       </c>
       <c r="AH65" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI65" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="AJ65" t="s">
         <v>757</v>
@@ -17463,7 +17463,7 @@
         <v>72016</v>
       </c>
       <c r="AL65" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="AM65" s="0">
         <v>1</v>
@@ -17477,13 +17477,13 @@
         <v>222</v>
       </c>
       <c r="B66" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C66" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D66" t="s">
-        <v>50</v>
+        <v>396</v>
       </c>
       <c r="E66" t="s">
         <v>411</v>
@@ -17540,13 +17540,13 @@
         <v>571</v>
       </c>
       <c r="Y66" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z66" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AA66" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="AB66" t="s">
         <v>633</v>
@@ -17558,19 +17558,19 @@
         <v>70746732</v>
       </c>
       <c r="AE66" s="0">
-        <v>14.033710479736328</v>
+        <v>14.029009819030762</v>
       </c>
       <c r="AF66" s="0">
-        <v>-0.031045390293002129</v>
+        <v>-0.032633930444717407</v>
       </c>
       <c r="AG66" s="0">
-        <v>301.39999389648437</v>
+        <v>304.89999389648438</v>
       </c>
       <c r="AH66" s="0">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AI66" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="AJ66" t="s">
         <v>757</v>
@@ -17579,7 +17579,7 @@
         <v>72016</v>
       </c>
       <c r="AL66" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="AM66" s="0">
         <v>1</v>
@@ -18065,13 +18065,13 @@
         <v>222</v>
       </c>
       <c r="B71" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C71" t="s">
-        <v>376</v>
+        <v>288</v>
       </c>
       <c r="D71" t="s">
-        <v>50</v>
+        <v>396</v>
       </c>
       <c r="E71" t="s">
         <v>411</v>
@@ -18127,16 +18127,16 @@
         <v>0</v>
       </c>
       <c r="X71" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="Y71" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z71" s="0">
         <v>3</v>
       </c>
       <c r="AA71" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="AB71" t="s">
         <v>633</v>
@@ -18148,19 +18148,19 @@
         <v>70746732</v>
       </c>
       <c r="AE71" s="0">
-        <v>14.033783912658691</v>
+        <v>14.029053688049316</v>
       </c>
       <c r="AF71" s="0">
-        <v>-0.031044170260429382</v>
+        <v>-0.03261445090174675</v>
       </c>
       <c r="AG71" s="0">
-        <v>303.79998779296875</v>
+        <v>308.5</v>
       </c>
       <c r="AH71" s="0">
         <v>5</v>
       </c>
       <c r="AI71" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="AJ71" t="s">
         <v>760</v>
@@ -18169,7 +18169,7 @@
         <v>72016</v>
       </c>
       <c r="AL71" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="AM71" s="0">
         <v>1</v>
@@ -18183,13 +18183,13 @@
         <v>222</v>
       </c>
       <c r="B72" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C72" t="s">
-        <v>288</v>
+        <v>376</v>
       </c>
       <c r="D72" t="s">
-        <v>396</v>
+        <v>50</v>
       </c>
       <c r="E72" t="s">
         <v>411</v>
@@ -18245,16 +18245,16 @@
         <v>0</v>
       </c>
       <c r="X72" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="Y72" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z72" s="0">
         <v>3</v>
       </c>
       <c r="AA72" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AB72" t="s">
         <v>633</v>
@@ -18266,19 +18266,19 @@
         <v>70746732</v>
       </c>
       <c r="AE72" s="0">
-        <v>14.029053688049316</v>
+        <v>14.033783912658691</v>
       </c>
       <c r="AF72" s="0">
-        <v>-0.03261445090174675</v>
+        <v>-0.031044170260429382</v>
       </c>
       <c r="AG72" s="0">
-        <v>308.5</v>
+        <v>303.79998779296875</v>
       </c>
       <c r="AH72" s="0">
         <v>5</v>
       </c>
       <c r="AI72" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="AJ72" t="s">
         <v>760</v>
@@ -18287,7 +18287,7 @@
         <v>72016</v>
       </c>
       <c r="AL72" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="AM72" s="0">
         <v>1</v>
@@ -21876,16 +21876,16 @@
         <v>214</v>
       </c>
       <c r="B16" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="C16" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="D16" t="s">
         <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F16" t="s">
         <v>65</v>
@@ -21906,13 +21906,13 @@
         <v>89</v>
       </c>
       <c r="L16" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="M16" s="0">
-        <v>78826743</v>
+        <v>72166910</v>
       </c>
       <c r="N16" s="0">
-        <v>78826743</v>
+        <v>72166910</v>
       </c>
       <c r="O16" s="0"/>
       <c r="P16" s="0">
@@ -21923,10 +21923,10 @@
         <v>2</v>
       </c>
       <c r="S16" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T16" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16" t="s">
         <v>130</v>
@@ -21938,19 +21938,19 @@
         <v>79146080</v>
       </c>
       <c r="X16" s="0">
-        <v>10.663545608520508</v>
+        <v>10.642724990844727</v>
       </c>
       <c r="Y16" s="0">
-        <v>-4.7367901802062988</v>
+        <v>-4.7599368095397949</v>
       </c>
       <c r="Z16" s="0">
-        <v>330.48666381835937</v>
+        <v>343.13467407226562</v>
       </c>
       <c r="AA16" s="0">
         <v>4</v>
       </c>
       <c r="AB16" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="AC16" t="s">
         <v>1316</v>
@@ -21959,7 +21959,7 @@
         <v>72016</v>
       </c>
       <c r="AE16" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="AF16" s="0">
         <v>1</v>
@@ -21973,16 +21973,16 @@
         <v>214</v>
       </c>
       <c r="B17" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C17" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D17" t="s">
         <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
         <v>65</v>
@@ -22003,13 +22003,13 @@
         <v>89</v>
       </c>
       <c r="L17" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="M17" s="0">
-        <v>72166910</v>
+        <v>78826743</v>
       </c>
       <c r="N17" s="0">
-        <v>72166910</v>
+        <v>78826743</v>
       </c>
       <c r="O17" s="0"/>
       <c r="P17" s="0">
@@ -22020,10 +22020,10 @@
         <v>2</v>
       </c>
       <c r="S17" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T17" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17" t="s">
         <v>130</v>
@@ -22035,19 +22035,19 @@
         <v>79146080</v>
       </c>
       <c r="X17" s="0">
-        <v>10.642724990844727</v>
+        <v>10.663545608520508</v>
       </c>
       <c r="Y17" s="0">
-        <v>-4.7599368095397949</v>
+        <v>-4.7367901802062988</v>
       </c>
       <c r="Z17" s="0">
-        <v>343.13467407226562</v>
+        <v>330.48666381835937</v>
       </c>
       <c r="AA17" s="0">
         <v>4</v>
       </c>
       <c r="AB17" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="AC17" t="s">
         <v>1316</v>
@@ -22056,7 +22056,7 @@
         <v>72016</v>
       </c>
       <c r="AE17" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="AF17" s="0">
         <v>1</v>
@@ -22458,13 +22458,13 @@
         <v>222</v>
       </c>
       <c r="B22" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C22" t="s">
-        <v>912</v>
+        <v>819</v>
       </c>
       <c r="D22" t="s">
-        <v>396</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s">
         <v>411</v>
@@ -22491,10 +22491,10 @@
         <v>1107</v>
       </c>
       <c r="M22" s="0">
-        <v>71296550</v>
+        <v>79942493</v>
       </c>
       <c r="N22" s="0">
-        <v>70028480</v>
+        <v>79942493</v>
       </c>
       <c r="O22" s="0"/>
       <c r="P22" s="0">
@@ -22508,7 +22508,7 @@
         <v>0</v>
       </c>
       <c r="T22" s="0">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="U22" t="s">
         <v>633</v>
@@ -22520,19 +22520,19 @@
         <v>70746732</v>
       </c>
       <c r="X22" s="0">
-        <v>14.029008865356445</v>
+        <v>14.036481857299805</v>
       </c>
       <c r="Y22" s="0">
-        <v>-0.032635558396577835</v>
+        <v>-0.032864119857549667</v>
       </c>
       <c r="Z22" s="0">
-        <v>306.39999389648437</v>
+        <v>305.60000610351562</v>
       </c>
       <c r="AA22" s="0">
         <v>5</v>
       </c>
       <c r="AB22" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="AC22" t="s">
         <v>1317</v>
@@ -22541,7 +22541,7 @@
         <v>72016</v>
       </c>
       <c r="AE22" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="AF22" s="0">
         <v>3</v>
@@ -22555,13 +22555,13 @@
         <v>222</v>
       </c>
       <c r="B23" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="C23" t="s">
-        <v>819</v>
+        <v>912</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>396</v>
       </c>
       <c r="E23" t="s">
         <v>411</v>
@@ -22588,10 +22588,10 @@
         <v>1107</v>
       </c>
       <c r="M23" s="0">
-        <v>79942493</v>
+        <v>71296550</v>
       </c>
       <c r="N23" s="0">
-        <v>79942493</v>
+        <v>70028480</v>
       </c>
       <c r="O23" s="0"/>
       <c r="P23" s="0">
@@ -22605,7 +22605,7 @@
         <v>0</v>
       </c>
       <c r="T23" s="0">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U23" t="s">
         <v>633</v>
@@ -22617,19 +22617,19 @@
         <v>70746732</v>
       </c>
       <c r="X23" s="0">
-        <v>14.036481857299805</v>
+        <v>14.029008865356445</v>
       </c>
       <c r="Y23" s="0">
-        <v>-0.032864119857549667</v>
+        <v>-0.032635558396577835</v>
       </c>
       <c r="Z23" s="0">
-        <v>305.60000610351562</v>
+        <v>306.39999389648437</v>
       </c>
       <c r="AA23" s="0">
         <v>5</v>
       </c>
       <c r="AB23" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="AC23" t="s">
         <v>1317</v>
@@ -22638,7 +22638,7 @@
         <v>72016</v>
       </c>
       <c r="AE23" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="AF23" s="0">
         <v>3</v>
@@ -25271,13 +25271,13 @@
         <v>782</v>
       </c>
       <c r="B51" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="C51" t="s">
-        <v>935</v>
+        <v>842</v>
       </c>
       <c r="D51" t="s">
-        <v>45</v>
+        <v>396</v>
       </c>
       <c r="E51" t="s">
         <v>411</v>
@@ -25301,13 +25301,13 @@
         <v>89</v>
       </c>
       <c r="L51" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="M51" s="0">
         <v>79867954</v>
       </c>
       <c r="N51" s="0">
-        <v>79867954</v>
+        <v>71296552</v>
       </c>
       <c r="O51" s="0"/>
       <c r="P51" s="0">
@@ -25315,16 +25315,16 @@
       </c>
       <c r="Q51" s="0"/>
       <c r="R51" s="0">
+        <v>3</v>
+      </c>
+      <c r="S51" s="0">
+        <v>1</v>
+      </c>
+      <c r="T51" s="0">
         <v>4</v>
       </c>
-      <c r="S51" s="0">
-        <v>1</v>
-      </c>
-      <c r="T51" s="0">
-        <v>5</v>
-      </c>
       <c r="U51" t="s">
-        <v>1174</v>
+        <v>633</v>
       </c>
       <c r="V51" s="0">
         <v>70746732</v>
@@ -25333,19 +25333,19 @@
         <v>70746732</v>
       </c>
       <c r="X51" s="0">
-        <v>14.036473274230957</v>
+        <v>14.02900505065918</v>
       </c>
       <c r="Y51" s="0">
-        <v>-0.03301481157541275</v>
+        <v>-0.032617561519145966</v>
       </c>
       <c r="Z51" s="0">
-        <v>308.29998779296875</v>
+        <v>305.5</v>
       </c>
       <c r="AA51" s="0">
         <v>5</v>
       </c>
       <c r="AB51" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="AC51" t="s">
         <v>1320</v>
@@ -25354,7 +25354,7 @@
         <v>72016</v>
       </c>
       <c r="AE51" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="AF51" s="0">
         <v>3</v>
@@ -25368,13 +25368,13 @@
         <v>782</v>
       </c>
       <c r="B52" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C52" t="s">
-        <v>842</v>
+        <v>935</v>
       </c>
       <c r="D52" t="s">
-        <v>396</v>
+        <v>45</v>
       </c>
       <c r="E52" t="s">
         <v>411</v>
@@ -25398,13 +25398,13 @@
         <v>89</v>
       </c>
       <c r="L52" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="M52" s="0">
         <v>79867954</v>
       </c>
       <c r="N52" s="0">
-        <v>71296552</v>
+        <v>79867954</v>
       </c>
       <c r="O52" s="0"/>
       <c r="P52" s="0">
@@ -25412,16 +25412,16 @@
       </c>
       <c r="Q52" s="0"/>
       <c r="R52" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S52" s="0">
         <v>1</v>
       </c>
       <c r="T52" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U52" t="s">
-        <v>633</v>
+        <v>1174</v>
       </c>
       <c r="V52" s="0">
         <v>70746732</v>
@@ -25430,19 +25430,19 @@
         <v>70746732</v>
       </c>
       <c r="X52" s="0">
-        <v>14.02900505065918</v>
+        <v>14.036473274230957</v>
       </c>
       <c r="Y52" s="0">
-        <v>-0.032617561519145966</v>
+        <v>-0.03301481157541275</v>
       </c>
       <c r="Z52" s="0">
-        <v>305.5</v>
+        <v>308.29998779296875</v>
       </c>
       <c r="AA52" s="0">
         <v>5</v>
       </c>
       <c r="AB52" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="AC52" t="s">
         <v>1320</v>
@@ -25451,7 +25451,7 @@
         <v>72016</v>
       </c>
       <c r="AE52" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="AF52" s="0">
         <v>3</v>
@@ -25853,13 +25853,13 @@
         <v>782</v>
       </c>
       <c r="B57" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C57" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="D57" t="s">
-        <v>45</v>
+        <v>396</v>
       </c>
       <c r="E57" t="s">
         <v>411</v>
@@ -25886,7 +25886,7 @@
         <v>1125</v>
       </c>
       <c r="M57" s="0">
-        <v>79664235</v>
+        <v>71296557</v>
       </c>
       <c r="N57" s="0">
         <v>79664235</v>
@@ -25897,13 +25897,13 @@
       </c>
       <c r="Q57" s="0"/>
       <c r="R57" s="0">
+        <v>2</v>
+      </c>
+      <c r="S57" s="0">
+        <v>1</v>
+      </c>
+      <c r="T57" s="0">
         <v>5</v>
-      </c>
-      <c r="S57" s="0">
-        <v>1</v>
-      </c>
-      <c r="T57" s="0">
-        <v>7</v>
       </c>
       <c r="U57" t="s">
         <v>633</v>
@@ -25915,19 +25915,19 @@
         <v>70746732</v>
       </c>
       <c r="X57" s="0">
-        <v>14.036609649658203</v>
+        <v>14.029008865356445</v>
       </c>
       <c r="Y57" s="0">
-        <v>-0.032943520694971085</v>
+        <v>-0.032592598348855972</v>
       </c>
       <c r="Z57" s="0">
-        <v>313.60000610351562</v>
+        <v>312.10000610351562</v>
       </c>
       <c r="AA57" s="0">
         <v>5</v>
       </c>
       <c r="AB57" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="AC57" t="s">
         <v>1320</v>
@@ -25936,7 +25936,7 @@
         <v>72016</v>
       </c>
       <c r="AE57" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="AF57" s="0">
         <v>3</v>
@@ -25950,13 +25950,13 @@
         <v>782</v>
       </c>
       <c r="B58" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C58" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="D58" t="s">
-        <v>396</v>
+        <v>45</v>
       </c>
       <c r="E58" t="s">
         <v>411</v>
@@ -25983,7 +25983,7 @@
         <v>1125</v>
       </c>
       <c r="M58" s="0">
-        <v>71296557</v>
+        <v>79664235</v>
       </c>
       <c r="N58" s="0">
         <v>79664235</v>
@@ -25994,13 +25994,13 @@
       </c>
       <c r="Q58" s="0"/>
       <c r="R58" s="0">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S58" s="0">
         <v>1</v>
       </c>
       <c r="T58" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="U58" t="s">
         <v>633</v>
@@ -26012,19 +26012,19 @@
         <v>70746732</v>
       </c>
       <c r="X58" s="0">
-        <v>14.029008865356445</v>
+        <v>14.036609649658203</v>
       </c>
       <c r="Y58" s="0">
-        <v>-0.032592598348855972</v>
+        <v>-0.032943520694971085</v>
       </c>
       <c r="Z58" s="0">
-        <v>312.10000610351562</v>
+        <v>313.60000610351562</v>
       </c>
       <c r="AA58" s="0">
         <v>5</v>
       </c>
       <c r="AB58" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="AC58" t="s">
         <v>1320</v>
@@ -26033,7 +26033,7 @@
         <v>72016</v>
       </c>
       <c r="AE58" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="AF58" s="0">
         <v>3</v>
@@ -26047,13 +26047,13 @@
         <v>776</v>
       </c>
       <c r="B59" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C59" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="D59" t="s">
-        <v>396</v>
+        <v>45</v>
       </c>
       <c r="E59" t="s">
         <v>411</v>
@@ -26080,10 +26080,10 @@
         <v>1125</v>
       </c>
       <c r="M59" s="0">
+        <v>79664235</v>
+      </c>
+      <c r="N59" s="0">
         <v>71296557</v>
-      </c>
-      <c r="N59" s="0">
-        <v>79664235</v>
       </c>
       <c r="O59" s="0"/>
       <c r="P59" s="0">
@@ -26091,13 +26091,13 @@
       </c>
       <c r="Q59" s="0"/>
       <c r="R59" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S59" s="0">
         <v>0</v>
       </c>
       <c r="T59" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="U59" t="s">
         <v>633</v>
@@ -26109,19 +26109,19 @@
         <v>70746732</v>
       </c>
       <c r="X59" s="0">
-        <v>14.029008865356445</v>
+        <v>14.036609649658203</v>
       </c>
       <c r="Y59" s="0">
-        <v>-0.032592598348855972</v>
+        <v>-0.032943520694971085</v>
       </c>
       <c r="Z59" s="0">
-        <v>312.10000610351562</v>
+        <v>313.60000610351562</v>
       </c>
       <c r="AA59" s="0">
         <v>5</v>
       </c>
       <c r="AB59" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="AC59" t="s">
         <v>1320</v>
@@ -26130,7 +26130,7 @@
         <v>72016</v>
       </c>
       <c r="AE59" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="AF59" s="0">
         <v>3</v>
@@ -26144,13 +26144,13 @@
         <v>776</v>
       </c>
       <c r="B60" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C60" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="D60" t="s">
-        <v>45</v>
+        <v>396</v>
       </c>
       <c r="E60" t="s">
         <v>411</v>
@@ -26177,10 +26177,10 @@
         <v>1125</v>
       </c>
       <c r="M60" s="0">
+        <v>71296557</v>
+      </c>
+      <c r="N60" s="0">
         <v>79664235</v>
-      </c>
-      <c r="N60" s="0">
-        <v>71296557</v>
       </c>
       <c r="O60" s="0"/>
       <c r="P60" s="0">
@@ -26188,13 +26188,13 @@
       </c>
       <c r="Q60" s="0"/>
       <c r="R60" s="0">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S60" s="0">
         <v>0</v>
       </c>
       <c r="T60" s="0">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="U60" t="s">
         <v>633</v>
@@ -26206,19 +26206,19 @@
         <v>70746732</v>
       </c>
       <c r="X60" s="0">
-        <v>14.036609649658203</v>
+        <v>14.029008865356445</v>
       </c>
       <c r="Y60" s="0">
-        <v>-0.032943520694971085</v>
+        <v>-0.032592598348855972</v>
       </c>
       <c r="Z60" s="0">
-        <v>313.60000610351562</v>
+        <v>312.10000610351562</v>
       </c>
       <c r="AA60" s="0">
         <v>5</v>
       </c>
       <c r="AB60" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="AC60" t="s">
         <v>1320</v>
@@ -26227,7 +26227,7 @@
         <v>72016</v>
       </c>
       <c r="AE60" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="AF60" s="0">
         <v>3</v>
@@ -30701,10 +30701,10 @@
         <v>782</v>
       </c>
       <c r="B107" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="C107" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="D107" t="s">
         <v>45</v>
@@ -30734,7 +30734,7 @@
         <v>1151</v>
       </c>
       <c r="M107" s="0">
-        <v>71296554</v>
+        <v>70035628</v>
       </c>
       <c r="N107" s="0">
         <v>71296554</v>
@@ -30763,19 +30763,19 @@
         <v>70746732</v>
       </c>
       <c r="X107" s="0">
-        <v>14.036513328552246</v>
+        <v>13.752680778503418</v>
       </c>
       <c r="Y107" s="0">
-        <v>-0.032899491488933563</v>
+        <v>0.21721181273460388</v>
       </c>
       <c r="Z107" s="0">
-        <v>303.5</v>
+        <v>307.39999389648437</v>
       </c>
       <c r="AA107" s="0">
         <v>5</v>
       </c>
       <c r="AB107" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="AC107" t="s">
         <v>1335</v>
@@ -30784,7 +30784,7 @@
         <v>72016</v>
       </c>
       <c r="AE107" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="AF107" s="0">
         <v>1</v>
@@ -30798,10 +30798,10 @@
         <v>782</v>
       </c>
       <c r="B108" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="C108" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="D108" t="s">
         <v>45</v>
@@ -30831,7 +30831,7 @@
         <v>1151</v>
       </c>
       <c r="M108" s="0">
-        <v>70035628</v>
+        <v>71296554</v>
       </c>
       <c r="N108" s="0">
         <v>71296554</v>
@@ -30860,19 +30860,19 @@
         <v>70746732</v>
       </c>
       <c r="X108" s="0">
-        <v>13.752680778503418</v>
+        <v>14.036513328552246</v>
       </c>
       <c r="Y108" s="0">
-        <v>0.21721181273460388</v>
+        <v>-0.032899491488933563</v>
       </c>
       <c r="Z108" s="0">
-        <v>307.39999389648437</v>
+        <v>303.5</v>
       </c>
       <c r="AA108" s="0">
         <v>5</v>
       </c>
       <c r="AB108" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="AC108" t="s">
         <v>1335</v>
@@ -30881,7 +30881,7 @@
         <v>72016</v>
       </c>
       <c r="AE108" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="AF108" s="0">
         <v>1</v>
@@ -32055,10 +32055,10 @@
         <v>775</v>
       </c>
       <c r="B121" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="C121" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="D121" t="s">
         <v>46</v>
@@ -32085,13 +32085,13 @@
         <v>89</v>
       </c>
       <c r="L121" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="M121" s="0">
-        <v>68463775</v>
+        <v>76493199</v>
       </c>
       <c r="N121" s="0">
-        <v>68463775</v>
+        <v>76493199</v>
       </c>
       <c r="O121" s="0"/>
       <c r="P121" s="0">
@@ -32105,7 +32105,7 @@
         <v>0</v>
       </c>
       <c r="T121" s="0">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U121" t="s">
         <v>130</v>
@@ -32117,19 +32117,19 @@
         <v>79146080</v>
       </c>
       <c r="X121" s="0">
-        <v>10.663528442382813</v>
+        <v>10.663491249084473</v>
       </c>
       <c r="Y121" s="0">
-        <v>-4.7367877960205078</v>
+        <v>-4.7367987632751465</v>
       </c>
       <c r="Z121" s="0">
-        <v>329.90121459960937</v>
+        <v>347.54165649414062</v>
       </c>
       <c r="AA121" s="0">
         <v>4</v>
       </c>
       <c r="AB121" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="AC121" t="s">
         <v>1341</v>
@@ -32138,7 +32138,7 @@
         <v>72016</v>
       </c>
       <c r="AE121" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="AF121" s="0">
         <v>1</v>
@@ -32152,10 +32152,10 @@
         <v>775</v>
       </c>
       <c r="B122" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="C122" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="D122" t="s">
         <v>46</v>
@@ -32182,13 +32182,13 @@
         <v>89</v>
       </c>
       <c r="L122" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="M122" s="0">
-        <v>76493199</v>
+        <v>68463775</v>
       </c>
       <c r="N122" s="0">
-        <v>76493199</v>
+        <v>68463775</v>
       </c>
       <c r="O122" s="0"/>
       <c r="P122" s="0">
@@ -32202,7 +32202,7 @@
         <v>0</v>
       </c>
       <c r="T122" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U122" t="s">
         <v>130</v>
@@ -32214,19 +32214,19 @@
         <v>79146080</v>
       </c>
       <c r="X122" s="0">
-        <v>10.663491249084473</v>
+        <v>10.663528442382813</v>
       </c>
       <c r="Y122" s="0">
-        <v>-4.7367987632751465</v>
+        <v>-4.7367877960205078</v>
       </c>
       <c r="Z122" s="0">
-        <v>347.54165649414062</v>
+        <v>329.90121459960937</v>
       </c>
       <c r="AA122" s="0">
         <v>4</v>
       </c>
       <c r="AB122" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="AC122" t="s">
         <v>1341</v>
@@ -32235,7 +32235,7 @@
         <v>72016</v>
       </c>
       <c r="AE122" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="AF122" s="0">
         <v>1</v>
@@ -32637,10 +32637,10 @@
         <v>806</v>
       </c>
       <c r="B127" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="C127" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="D127" t="s">
         <v>45</v>
@@ -32681,16 +32681,16 @@
       </c>
       <c r="Q127" s="0"/>
       <c r="R127" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S127" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T127" s="0">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U127" t="s">
-        <v>628</v>
+        <v>1186</v>
       </c>
       <c r="V127" s="0">
         <v>71938391</v>
@@ -32699,19 +32699,19 @@
         <v>75448501</v>
       </c>
       <c r="X127" s="0">
-        <v>12.245701789855957</v>
+        <v>12.245555877685547</v>
       </c>
       <c r="Y127" s="0">
-        <v>-0.60631304979324341</v>
+        <v>-0.60626500844955444</v>
       </c>
       <c r="Z127" s="0">
-        <v>336.67626953125</v>
+        <v>374.84298706054687</v>
       </c>
       <c r="AA127" s="0">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="AB127" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="AC127" t="s">
         <v>1344</v>
@@ -32720,7 +32720,7 @@
         <v>72016</v>
       </c>
       <c r="AE127" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="AF127" s="0">
         <v>1</v>
@@ -32734,10 +32734,10 @@
         <v>806</v>
       </c>
       <c r="B128" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="C128" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="D128" t="s">
         <v>45</v>
@@ -32778,16 +32778,16 @@
       </c>
       <c r="Q128" s="0"/>
       <c r="R128" s="0">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S128" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T128" s="0">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U128" t="s">
-        <v>1186</v>
+        <v>628</v>
       </c>
       <c r="V128" s="0">
         <v>71938391</v>
@@ -32796,19 +32796,19 @@
         <v>75448501</v>
       </c>
       <c r="X128" s="0">
-        <v>12.245555877685547</v>
+        <v>12.245701789855957</v>
       </c>
       <c r="Y128" s="0">
-        <v>-0.60626500844955444</v>
+        <v>-0.60631304979324341</v>
       </c>
       <c r="Z128" s="0">
-        <v>374.84298706054687</v>
+        <v>336.67626953125</v>
       </c>
       <c r="AA128" s="0">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="AB128" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="AC128" t="s">
         <v>1344</v>
@@ -32817,7 +32817,7 @@
         <v>72016</v>
       </c>
       <c r="AE128" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="AF128" s="0">
         <v>1</v>

</xml_diff>